<commit_message>
[Add, Fix] contributions calculation and gpt analysis
</commit_message>
<xml_diff>
--- a/prompting/prompts.xlsx
+++ b/prompting/prompts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bidcompanysrl-my.sharepoint.com/personal/giorgio_barazzetta_bidcompany_it/Documents/Desktop/Lavori/BPER/bper-xai4clo/prompting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{2A505184-53F2-4D7E-A16B-4B294EC6CBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8EC5460-DB30-4442-8359-6098ED798548}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{2A505184-53F2-4D7E-A16B-4B294EC6CBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B758FDE9-7A5B-4474-8315-43AB3AA30A51}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15270" xr2:uid="{FB37A516-BB44-42E9-9458-7A7804F4201A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FB37A516-BB44-42E9-9458-7A7804F4201A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="20240201" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
   <si>
     <t>setup</t>
   </si>
@@ -517,6 +518,1225 @@
 Inoltre, il "Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)" ha un valore di -0.07, suggerendo che il cliente è stato in grado di mantenere i pagamenti delle rate, un segnale positivo.
 In sintesi, sembra che il cliente stia mostrando alcuni segnali di potenziale difficoltà finanziaria, come l'uso eccessivo del credito e il superamento del limite del conto corrente. Tuttavia, ci sono anche alcuni segnali positivi, come il mantenimento di un saldo minimo relativamente alto e il pagamento regolare delle rate. Questi fattori combinati suggeriscono un rischio moderato di insolvenza.</t>
   </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo, in termini di SHAP-value, di ogni variabile alla previsione di un tuo modello di classificazione.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente.
+Fornisci una spiegazione della previsione svolta dal modello, secondo il seguente schema:
+- Variabili che hanno influenzato positivamente la previsione.
+- Variabili che hanno influenzato negativamente la previsione. 
+- I comportamenti del cliente che si possono dedurre analizzando le variabili che hanno contribuito maggiormente.
+Concludi riassumendo le evidenze che hai trovato.
+&lt;table&gt;
+| Descrizione                                                                                                     |   SHAP_values |
+|:----------------------------------------------------------------------------------------------------------------|--------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |         0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |         0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |        -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |         0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |         0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |        -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |         0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |         0.322 |
+| utilizzo su accordato revoca snb                                                                                |         0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |         0.267 |
+| sconfino scadenza su margine scadenza                                                                           |        -0.002 |
+| utilizzato cassa su fatturato                                                                                   |        -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |        -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |         0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |         0.116 |
+| Copertura dell'indebitamento                                                                                    |         0.116 |
+| Debiti bancari su ricavi netti                                                                                  |         0.014 |
+| Valore debiti commerciali                                                                                       |         0.007 |
+| Liquidità su attivo netto                                                                                       |         0.046 |
+| Utile su ricavi                                                                                                 |         0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |        -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |        -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |         0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |         0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |         0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |        -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Variabili che hanno influenzato positivamente la previsione:
+- Somma Utilizzato su Somma Accordato negli ultimi due mesi
+- Media Giorni di Disponibilità CC negli ultimi tre mesi
+- Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+- Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+- Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+- Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+- Utilizzo su accordato revoca snb
+- Utilizzo su accordato autoliquidante snb
+- Sconfino medio revoca &gt; 1000€
+- Utilizzo firma finanziaria su accordato firma finanziaria
+- Copertura dell'indebitamento
+- Debiti bancari su ricavi netti
+- Valore debiti commerciali
+- Liquidità su attivo netto
+- Utile su ricavi
+- Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+- Importo mediano della somma entrate settimanali delle ultime 52 settimane
+- PD media ufficiale nell’ultimo mese
+Variabili che hanno influenzato negativamente la previsione:
+- Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+- Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+- Sconfino scadenza su margine scadenza
+- Utilizzato cassa su fatturato
+- Factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+- Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+- Regolarità mensile nel pagamento di prestiti e finanziamenti
+- Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+Comportamenti del cliente:
+Il cliente sembra avere un comportamento finanziario piuttosto attivo, con un alto livello di utilizzo del credito accordato e un numero significativo di giorni di sconfino. Tuttavia, il cliente ha anche mostrato segni di irregolarità nei pagamenti e un livello di allerta complessivo.
+In conclusione, il modello sembra indicare che il cliente ha un comportamento finanziario attivo ma con alcuni segni di rischio. Le variabili che hanno contribuito maggiormente alla previsione sono legate all'utilizzo del credito e alla gestione del debito.</t>
+  </si>
+  <si>
+    <t>1min 26s</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo, in termini di SHAP-value, di ogni variabile alla previsione di un tuo modello di classificazione.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente.
+Fornisci una spiegazione della previsione svolta dal modello, secondo il seguente schema:
+- Variabili più rilevanti che hanno influenzato positivamente la previsione.
+- Variabili più rilevanti che hanno influenzato negativamente la previsione. 
+- I comportamenti del cliente che si possono dedurre analizzando le variabili che hanno contribuito maggiormente.
+Concludi riassumendo le evidenze che hai trovato.
+&lt;table&gt;
+| Descrizione                                                                                                     |   SHAP_values |
+|:----------------------------------------------------------------------------------------------------------------|--------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |         0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |         0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |        -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |         0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |         0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |        -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |         0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |         0.322 |
+| utilizzo su accordato revoca snb                                                                                |         0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |         0.267 |
+| sconfino scadenza su margine scadenza                                                                           |        -0.002 |
+| utilizzato cassa su fatturato                                                                                   |        -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |        -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |         0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |         0.116 |
+| Copertura dell'indebitamento                                                                                    |         0.116 |
+| Debiti bancari su ricavi netti                                                                                  |         0.014 |
+| Valore debiti commerciali                                                                                       |         0.007 |
+| Liquidità su attivo netto                                                                                       |         0.046 |
+| Utile su ricavi                                                                                                 |         0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |        -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |        -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |         0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |         0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |         0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |        -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>ha riportato troppe variabili</t>
+  </si>
+  <si>
+    <t>Le variabili che hanno influenzato positivamente la previsione sono:
+- "Somma Utilizzato su Somma Accordato negli ultimi due mesi" con un SHAP value di 0.396. Questo indica che il cliente ha utilizzato una grande parte del suo credito accordato, il che potrebbe indicare un buon comportamento di rimborso.
+- "Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi" con un SHAP value di 0.257. Questo suggerisce che il cliente ha avuto un numero relativamente basso di giorni in cui ha superato il suo limite di credito, il che è un segno positivo.
+- "Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata" con un SHAP value di 0.207. Questo indica che il cliente ha avuto un importo massimo di sconfino superiore a 100 nell'ultimo mese, il che potrebbe indicare un buon comportamento di rimborso.
+- "Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi" con un SHAP value di 0.322. Questo suggerisce che il cliente ha un basso importo di effetti trassati insoluti rispetto agli effetti scaduti, il che è un segno positivo.
+Le variabili che hanno influenzato negativamente la previsione sono:
+- "Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi" con un SHAP value di -0.1. Questo indica che il cliente ha utilizzato una grande parte del suo credito rispetto alla sua giacenza minima, il che potrebbe indicare un rischio di insolvenza.
+- "Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)" con un SHAP value di -0.07. Questo suggerisce che il cliente ha avuto un numero elevato di rate impagate, il che è un segno negativo.
+- "sconfino scadenza su margine scadenza" con un SHAP value di -0.002. Questo indica che il cliente ha avuto un alto sconfino rispetto al margine di scadenza, il che potrebbe indicare un rischio di insolvenza.
+- "Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre" con un SHAP value di -0.027. Questo suggerisce che c'è stata una variazione negativa tra il tasso di default previsto e quello osservato, il che è un segno negativo.
+Analizzando le variabili che hanno contribuito maggiormente, si può dedurre che il cliente ha un buon comportamento di rimborso, ma presenta alcuni segni di rischio di insolvenza. In particolare, il cliente ha utilizzato una grande parte del suo credito accordato e ha avuto un numero relativamente basso di giorni in cui ha superato il suo limite di credito. Tuttavia, il cliente ha anche utilizzato una grande parte del suo credito rispetto alla sua giacenza minima e ha avuto un numero elevato di rate impagate.
+In conclusione, le evidenze suggeriscono che il cliente ha un comportamento di rimborso generalmente buono, ma presenta alcuni segni di rischio. Questo suggerisce che potrebbe essere necessario monitorare attentamente il comportamento del cliente e prendere eventuali misure preventive per mitigare il rischio di insolvenza.</t>
+  </si>
+  <si>
+    <t>Non imputare il comportamento dai valori shap</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo, in termini di SHAP-value, di ogni variabile alla previsione di un tuo modello di classificazione.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente.
+Fornisci una spiegazione della previsione svolta dal modello, secondo il seguente schema:
+- Variabili più rilevanti che hanno influenzato positivamente la previsione.
+- Variabili più rilevanti che hanno influenzato negativamente la previsione. 
+- I comportamenti del cliente che si possono dedurre analizzando le variabili che hanno contribuito maggiormente.
+Concludi riassumendo le evidenze che hai trovato.
+Alcune note:
+- Previsione prositiva del modello indica cliente con alta rischiosità.
+- Utilizza i valori shap solo per identificare quali sono le variabili più rilevanti.
+- Il comportamento deve essere dedotto aggregando variabili di natura simile e rilevanti per il modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   SHAP_values |
+|:----------------------------------------------------------------------------------------------------------------|--------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |         0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |         0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |        -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |         0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |         0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |        -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |         0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |         0.322 |
+| utilizzo su accordato revoca snb                                                                                |         0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |         0.267 |
+| sconfino scadenza su margine scadenza                                                                           |        -0.002 |
+| utilizzato cassa su fatturato                                                                                   |        -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |        -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |         0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |         0.116 |
+| Copertura dell'indebitamento                                                                                    |         0.116 |
+| Debiti bancari su ricavi netti                                                                                  |         0.014 |
+| Valore debiti commerciali                                                                                       |         0.007 |
+| Liquidità su attivo netto                                                                                       |         0.046 |
+| Utile su ricavi                                                                                                 |         0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |        -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |        -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |         0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |         0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |         0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |        -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Variabili più rilevanti che hanno influenzato positivamente la previsione:
+- Somma Utilizzato su Somma Accordato negli ultimi due mesi (0.396)
+- Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi (0.257)
+- Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata (0.207)
+- Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi (0.322)
+- Utilizzo su accordato revoca snb (0.308)
+- Utilizzo su accordato autoliquidante snb (0.267)
+- Sconfino medio revoca &gt; 1000€ (0.183)
+- Utilizzo firma finanziaria su accordato firma finanziaria (0.116)
+- Copertura dell'indebitamento (0.116)
+- Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente (0.174)
+- PD media ufficiale nell’ultimo mese (0.261)
+Variabili più rilevanti che hanno influenzato negativamente la previsione:
+- Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi (-0.1)
+- Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui) (-0.07)
+- Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre (-0.027)
+Comportamenti del cliente dedotti:
+- Il cliente ha un alto utilizzo del credito rispetto a quanto gli è stato accordato, indicando un possibile sovraindebitamento.
+- Il cliente ha avuto un numero significativo di giorni di sconfino (ovvero ha superato il limite del suo conto corrente) negli ultimi sei mesi.
+- Il cliente ha avuto un importo di sconfino superiore a 100 nell'ultimo mese.
+- Il cliente ha un alto numero di effetti trassati insoluti rispetto agli effetti scaduti negli ultimi tre mesi.
+- Il cliente ha un alto utilizzo del credito rispetto a quanto gli è stato accordato sia per la revoca snb che per l'autoliquidante snb.
+- Il cliente ha un alto livello di indebitamento rispetto alla sua capacità di copertura.
+- Il cliente ha un alto livello di movimentazione del conto corrente, sia in termini di numero che di importi dei movimenti.
+- Il cliente ha un alto PD (Probability of Default) medio nell'ultimo mese.
+In conclusione, il modello indica che il cliente ha un alto rischio di default, principalmente a causa del suo alto livello di utilizzo del credito, del numero di giorni di sconfino, del numero di effetti trassati insoluti e del suo alto livello di indebitamento rispetto alla sua capacità di copertura.</t>
+  </si>
+  <si>
+    <t>1min 25s</t>
+  </si>
+  <si>
+    <t>Non fa quanto richiesto</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo, in termini di SHAP-value, di ogni variabile alla previsione di un tuo modello di classificazione.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente.
+Fornisci una spiegazione della previsione svolta dal modello, secondo il seguente schema:
+- Variabili più rilevanti che hanno influenzato positivamente la previsione (ordinamento descrescente).
+- Variabili più rilevanti che hanno influenzato negativamente la previsione (ordinamento crescente). 
+- I comportamenti del cliente che si possono dedurre analizzando le variabili che hanno contribuito maggiormente.
+Concludi riassumendo le evidenze che hai trovato.
+Alcune note:
+- Previsione prositiva del modello indica cliente con alta rischiosità.
+- Utilizza i valori shap solo per identificare quali sono le variabili più rilevanti.
+- Il comportamento deve essere dedotto aggregando variabili di natura simile e rilevanti per il modello.
+- Nel costruire la risposta non fare riferimento ai valori shap.
+- La struttura del comportamento deve essere: dato che "variabile A" e "variabile B" sono positive allora il cliente ha questo comportamento.
+&lt;table&gt;
+| Descrizione                                                                                                     |   SHAP_values |
+|:----------------------------------------------------------------------------------------------------------------|--------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |         0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |         0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |        -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |         0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |         0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |        -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |         0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |         0.322 |
+| utilizzo su accordato revoca snb                                                                                |         0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |         0.267 |
+| sconfino scadenza su margine scadenza                                                                           |        -0.002 |
+| utilizzato cassa su fatturato                                                                                   |        -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |        -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |         0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |         0.116 |
+| Copertura dell'indebitamento                                                                                    |         0.116 |
+| Debiti bancari su ricavi netti                                                                                  |         0.014 |
+| Valore debiti commerciali                                                                                       |         0.007 |
+| Liquidità su attivo netto                                                                                       |         0.046 |
+| Utile su ricavi                                                                                                 |         0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |        -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |        -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |         0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |         0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |         0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |        -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>1min 27s</t>
+  </si>
+  <si>
+    <t>Variabili più rilevanti che hanno influenzato positivamente la previsione:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. Utilizzo su accordato revoca snb
+4. Utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+9. Utilizzo firma finanziaria su accordato firma finanziaria
+10. Copertura dell'indebitamento
+Variabili più rilevanti che hanno influenzato negativamente la previsione:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Utilizzato cassa su fatturato
+4. Factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+Comportamenti del cliente:
+- Il cliente ha un alto utilizzo del credito accordato, sia in termini di somma utilizzata rispetto alla somma accordata negli ultimi due mesi, sia in termini di utilizzo su accordato revoca e autoliquidante snb. Questo indica un comportamento di elevato utilizzo del credito disponibile.
+- Il cliente ha avuto un alto numero di giorni di sconfino negli ultimi sei mesi e un massimo importo di sconfino superiore a 100 nell'ultimo mese. Questo indica un comportamento di sconfino frequente.
+- Il cliente ha avuto un alto importo di effetti trassati insoluti e di effetti protestati o richiamati rispetto agli effetti scaduti negli ultimi mesi. Questo indica un comportamento di mancato pagamento degli effetti.
+- Il cliente ha un basso rapporto tra la somma utilizzata e la somma giacenza minima negli ultimi due mesi e un alto numero di rate impagate negli ultimi tre mesi. Questo indica un comportamento di difficoltà nel gestire i propri debiti.
+In conclusione, il modello ha identificato un cliente con un comportamento di elevato utilizzo del credito, frequenti sconfini e difficoltà nel gestire i propri debiti. Questi comportamenti hanno contribuito a una previsione di alta rischiosità per il cliente.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo, in termini di SHAP-value, di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili che hanno incrementato la rischiosità del cliente ordinate in maniera decrescente.
+- Lista variabili che hanno diminuito la rischiosità del cliente ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e deduci la tipologia di comportamento. Il contributo rappresenta l'importanza della variabile non il suo valore.
+[Conclusione]
+Riassumi le evidenze che hai trovato.
+&lt;table&gt;
+| Descrizione                                                                                                     |   SHAP_values |
+|:----------------------------------------------------------------------------------------------------------------|--------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |         0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |         0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |        -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |         0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |         0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |        -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |         0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |         0.322 |
+| utilizzo su accordato revoca snb                                                                                |         0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |         0.267 |
+| sconfino scadenza su margine scadenza                                                                           |        -0.002 |
+| utilizzato cassa su fatturato                                                                                   |        -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |        -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |         0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |         0.116 |
+| Copertura dell'indebitamento                                                                                    |         0.116 |
+| Debiti bancari su ricavi netti                                                                                  |         0.014 |
+| Valore debiti commerciali                                                                                       |         0.007 |
+| Liquidità su attivo netto                                                                                       |         0.046 |
+| Utile su ricavi                                                                                                 |         0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |        -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |        -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |         0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |         0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |         0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |        -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Variabili che hanno incrementato la rischiosità del cliente (in ordine decrescente):
+- Somma Utilizzato su Somma Accordato negli ultimi due mesi
+- Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+- Utilizzo su accordato revoca snb
+- Utilizzo su accordato autoliquidante snb
+- Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+- Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+- PD media ufficiale nell’ultimo mese
+- Utilizzo firma finanziaria su accordato firma finanziaria
+- Copertura dell'indebitamento
+- Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+- Sconfino medio revoca &gt; 1000€
+- Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+- Importo mediano della somma entrate settimanali delle ultime 52 settimane
+- Media Giorni di Disponibilità CC negli ultimi tre mesi
+Variabili che hanno diminuito la rischiosità del cliente (in ordine crescente):
+- Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+- Factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+- Utilizzato cassa su fatturato
+- Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+- Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+- Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+[Comportamento cliente]:
+Il cliente sembra avere un comportamento finanziario rischioso. Ha un alto utilizzo del credito rispetto all'importo accordato, ha avuto un numero significativo di giorni di sconfino e ha un alto importo di effetti trassati insoluti. Inoltre, ha un alto livello di indebitamento e un basso livello di copertura dell'indebitamento. Tuttavia, ha un basso numero di rate impagate e un basso utilizzo della cassa rispetto al fatturato, il che potrebbe indicare una certa capacità di gestire i propri debiti.
+[Conclusione]
+Il modello suggerisce che il cliente ha un comportamento finanziario rischioso, con un alto livello di utilizzo del credito, un alto numero di giorni di sconfino e un alto livello di indebitamento. Tuttavia, ha anche alcuni fattori che potrebbero mitigare questo rischio, come un basso numero di rate impagate e un basso utilizzo della cassa rispetto al fatturato. Questi risultati suggeriscono che potrebbe essere necessario monitorare attentamente il comportamento finanziario di questo cliente e prendere in considerazione misure per mitigare il rischio.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista delle top 10 variabili che hanno incrementato la rischiosità del cliente ordinate in maniera decrescente.
+- Lista delle top 10 variabili che hanno diminuito la rischiosità del cliente ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e deduci i fattori principali che hanno determinato la previsione del modello.
+[Conclusione]
+Riassumi le evidenze che hai trovato.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e deduci il comportamento del cliente.
+[Conclusione]
+Riassumi le evidenze che hai trovato.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Variabili con contributo positivo ordinate in maniera decrescente:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. utilizzo firma finanziaria su accordato firma finanziaria
+9. Copertura dell'indebitamento
+10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Variabili con contributo negativo ordinate in maniera crescente:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. utilizzato cassa su fatturato
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+1. Utilizzo del credito: Questo gruppo include variabili come "Somma Utilizzato su Somma Accordato negli ultimi due mesi", "utilizzo su accordato revoca snb", "utilizzo su accordato autoliquidante snb" e "utilizzo firma finanziaria su accordato firma finanziaria". Queste variabili indicano che il cliente ha un alto utilizzo del credito rispetto a quanto gli è stato accordato.
+2. Gestione del debito: Questo gruppo include variabili come "Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi", "Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata" e "PD media ufficiale nell’ultimo mese". Queste variabili indicano che il cliente ha problemi nel gestire i suoi debiti.
+3. Comportamento di pagamento: Questo gruppo include variabili come "Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi" e "Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)". Queste variabili indicano che il cliente ha un comportamento di pagamento irregolare.
+[Conclusione]
+Il modello indica che il cliente ha un alto utilizzo del credito rispetto a quanto gli è stato accordato, ha problemi nel gestire i suoi debiti e ha un comportamento di pagamento irregolare. Questi fattori contribuiscono ad aumentare il rischio di credito del cliente.</t>
+  </si>
+  <si>
+    <t>1min 28s</t>
+  </si>
+  <si>
+    <t>modificare le conclusioni</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo.
+- Nome: &lt;Nome gruppo&gt;
+- Variabili: &lt;Lista variabili presenti&gt;
+- Significato: &lt;spiegazione del tipo di comportamento associato alle variabili presenti&gt;
+[Conclusione]
+Utilizza il significato di ogni gruppo che hai costruito per indicare quali comportamenti sono più evidenti.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Variabili con contributo positivo ordinate in maniera decrescente:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. sconfino medio revoca &gt; 1000€
+9. Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+10. utilizzo firma finanziaria su accordato firma finanziaria
+Variabili con contributo negativo ordinate in maniera crescente:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. utilizzato cassa su fatturato
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Significato: Queste variabili indicano l'uso del credito da parte del cliente. Un contributo positivo suggerisce che un maggiore utilizzo del credito è associato a un rischio maggiore.
+Nome: Sconfino
+Variabili: Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, sconfino medio revoca &gt; 1000€
+Significato: Queste variabili indicano l'entità e la frequenza con cui il cliente ha superato il limite di credito. Un contributo positivo suggerisce che un maggiore sconfino è associato a un rischio maggiore.
+Nome: Pagamenti
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui), Regolarità mensile nel pagamento di prestiti e finanziamenti
+Significato: Queste variabili indicano la regolarità dei pagamenti del cliente. Un contributo negativo suggerisce che una maggiore irregolarità nei pagamenti è associata a un rischio maggiore.
+[Conclusione]
+Il modello suggerisce che i comportamenti più rischiosi sono un elevato utilizzo del credito e frequenti sconfini. Inoltre, l'irregolarità nei pagamenti è associata a un rischio maggiore.</t>
+  </si>
+  <si>
+    <t>1min 8s</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo.
+- Nome: &lt;Nome gruppo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Significato: &lt;spiegazione del tipo di comportamento associato alle variabili presenti&gt;
+[Conclusione]
+Utilizza il significato di ogni gruppo per indicare come le variabili hanno influenzato la previsione.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Variabili con contributo positivo ordinate in maniera decrescente:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. utilizzo firma finanziaria su accordato firma finanziaria
+9. Copertura dell'indebitamento
+10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Variabili con contributo negativo ordinate in maniera crescente:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. utilizzato cassa su fatturato
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Significato: Queste variabili indicano come il cliente utilizza il credito a sua disposizione. Un alto utilizzo può indicare un rischio maggiore.
+Nome: Gestione del debito
+Variabili: Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, Copertura dell'indebitamento, Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Significato: Queste variabili indicano come il cliente gestisce i suoi debiti. Un alto numero di debiti insoluti o un alto importo di sconfino possono indicare un rischio maggiore.
+Nome: Rischi finanziari
+Variabili: PD media ufficiale nell’ultimo mese, Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+Significato: Queste variabili indicano il rischio finanziario associato al cliente. Un alto PD o un alto numero di rate impagate possono indicare un rischio maggiore.
+[Conclusione]
+Il modello indica che il cliente ha un alto rischio di default. Questo è dovuto principalmente all'alto utilizzo del credito, alla cattiva gestione del debito e al rischio finanziario associato. Il cliente dovrebbe cercare di migliorare la gestione del suo debito e ridurre il suo utilizzo del credito per ridurre il suo rischio di default.</t>
+  </si>
+  <si>
+    <t>1 min 45s</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta il contributo di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo. Crea almeno un gruppo per tipologia di contributo.
+- Nome: &lt;Nome gruppo&gt;
+- Tipologia: &lt;positivo o negativo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Significato: &lt;spiegazione del tipo di comportamento associato alle variabili del gruppo&gt;
+[Conclusione]
+Utilizza il significato di ogni gruppo per spiegare qualitativamente la previsione del modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Variabili con contributo positivo ordinate in maniera decrescente:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. utilizzo firma finanziaria su accordato firma finanziaria
+9. Copertura dell'indebitamento
+10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Variabili con contributo negativo ordinate in maniera crescente:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. utilizzato cassa su fatturato
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Tipologia: Positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Significato: Questo gruppo di variabili indica un utilizzo elevato del credito da parte del cliente, il che può indicare un rischio maggiore di insolvenza.
+Nome: Gestione del debito
+Tipologia: Negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui), Regolarità mensile nel pagamento di prestiti e finanziamenti
+Significato: Questo gruppo di variabili indica una gestione del debito non ottimale da parte del cliente, con un alto numero di rate impagate e una bassa regolarità nei pagamenti.
+[Conclusione]
+Il modello prevede un rischio di insolvenza più elevato per i clienti che utilizzano in modo intensivo il credito e che hanno una gestione del debito non ottimale. Al contrario, i clienti che gestiscono bene il loro debito e utilizzano il credito in modo moderato sono considerati meno rischiosi.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta l'importanza di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo. Crea almeno un gruppo per tipologia di contributo.
+- Nome: &lt;Nome gruppo&gt;
+- Tipologia: &lt;positivo o negativo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Significato: &lt;spiegazione del criterio utilizzato per la costruzione del gruppo&gt;
+[Conclusione]
+Utilizza il significato di ogni gruppo per spiegare qualitativamente la previsione del modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Contributo positivo:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. utilizzo firma finanziaria su accordato firma finanziaria
+9. Copertura dell'indebitamento
+10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Contributo negativo:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. utilizzato cassa su fatturato
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Tipologia: Positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Significato: Questo gruppo di variabili indica l'uso del credito da parte del cliente. Un contributo positivo suggerisce che un maggiore utilizzo del credito è associato a un rischio maggiore.
+Nome: Inadempimenti
+Tipologia: Negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+Significato: Questo gruppo di variabili indica l'inadempimento del cliente. Un contributo negativo suggerisce che un maggiore inadempimento è associato a un rischio minore.
+[Conclusione]
+Il modello suggerisce che i clienti che utilizzano di più il loro credito tendono ad essere più rischiosi. Al contrario, i clienti che hanno un alto livello di inadempimento tendono ad essere meno rischiosi. Questo potrebbe essere dovuto al fatto che i clienti che inadempiono sono più propensi a essere sottoposti a procedure di recupero del credito, riducendo così il rischio per la banca.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta l'importanza di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo.
+- Nome: &lt;Nome gruppo&gt;
+- Tipologia: &lt;positivo o negativo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Criterio: &lt;spiegazione del criterio utilizzato per la costruzione del gruppo&gt;
+[Conclusione]
+Utilizza il criterio di ogni gruppo per spiegare qualitativamente la previsione del modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Contributo positivo:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. PD media ufficiale nell’ultimo mese
+6. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+7. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+8. sconfino medio revoca &gt; 1000€
+9. Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+10. utilizzo firma finanziaria su accordato firma finanziaria
+Contributo negativo:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. utilizzato cassa su fatturato
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Tipologia: Positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Criterio: Queste variabili indicano l'uso del credito da parte del cliente. Un alto utilizzo del credito può indicare un rischio maggiore.
+Nome: Sconfino
+Tipologia: Positivo
+Variabili: Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, sconfino medio revoca &gt; 1000€
+Criterio: Queste variabili indicano il comportamento di sconfino del cliente. Un alto livello di sconfino può indicare un rischio maggiore.
+Nome: Pagamenti in ritardo
+Tipologia: Negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui), Regolarità mensile nel pagamento di prestiti e finanziamenti
+Criterio: Queste variabili indicano i ritardi nei pagamenti da parte del cliente. I ritardi nei pagamenti possono indicare un rischio minore.
+[Conclusione]
+Il modello prevede un rischio maggiore per i clienti che utilizzano molto il loro credito e che hanno un alto livello di sconfino. D'altra parte, prevede un rischio minore per i clienti che hanno ritardi nei pagamenti. Questo potrebbe essere dovuto al fatto che i clienti che utilizzano molto il loro credito o che hanno un alto livello di sconfino potrebbero avere difficoltà finanziarie, mentre i clienti che hanno ritardi nei pagamenti potrebbero essere più attenti nella gestione delle loro finanze.</t>
+  </si>
+  <si>
+    <t>1 min 36s</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta l'importanza di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo.
+- Nome: &lt;Nome gruppo&gt;
+- Tipologia: &lt;positivo o negativo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Criterio: &lt;Indica il criterio utilizzato per la costruzione del gruppo&gt;
+[Conclusione]
+Utilizza il criterio di ogni gruppo per spiegare qualitativamente come ciascun gruppo ha contribuito alla previsione del modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Contributo positivo:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. sconfino medio revoca &gt; 1000€
+8. Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+9. PD media ufficiale nell’ultimo mese
+10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+Contributo negativo:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. utilizzato cassa su fatturato
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Tipologia: Positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb
+Criterio: Variabili che indicano l'utilizzo del credito da parte del cliente.
+Nome: Sconfino
+Tipologia: Positivo
+Variabili: Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, sconfino medio revoca &gt; 1000€
+Criterio: Variabili che indicano il comportamento di sconfino del cliente.
+Nome: Pagamenti irregolari
+Tipologia: Negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+Criterio: Variabili che indicano irregolarità nei pagamenti del cliente.
+[Conclusione]
+Il modello indica che un alto utilizzo del credito e un comportamento di sconfino frequente sono associati a un rischio maggiore. D'altra parte, i pagamenti irregolari sono associati a un rischio minore. Questo suggerisce che i clienti che utilizzano molto il loro credito e che sconfinano frequentemente sono più propensi a essere classificati come rischiosi dal modello. Al contrario, i clienti che hanno un comportamento di pagamento irregolare sono meno propensi a essere classificati come rischiosi.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora per una banca. La tabella compresa tra i tag &lt;table&gt; riporta l'importanza di ogni variabile alla previsione di un tuo modello di rischiosità.
+Ogni variabile rappresenta una caratteristica del comportamento di un cliente. 
+Spiega la previsione svolta dal modello secondo il seguente schema:
+[Variabili rilevanti]:
+- Lista variabili (massimo 10) con contributo positivo ordinate in maniera decrescente.
+- Lista variabili (massimo 10) con contributo negativo ordinate in maniera crescente.
+[Comportamento cliente]:
+Raggruppa le variabili rilevanti con natura simile e contributo coerente. Nomina ciascun gruppo e spiega il significato del gruppo.
+- Nome: &lt;Nome gruppo&gt;
+- Tipologia: &lt;positivo o negativo&gt;
+- Variabili: &lt;Elenco variabili presenti&gt;
+- Criterio: &lt;Indica il criterio utilizzato per la costruzione del gruppo&gt;
+[Conclusione]
+Utilizza i gruppi come fattori per spiegare la previsione del modello.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>[Variabili rilevanti]:
+Contributo positivo:
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. PD media ufficiale nell’ultimo mese
+8. sconfino medio revoca &gt; 1000€
+9. Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+10. Copertura dell'indebitamento
+Contributo negativo:
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. utilizzato cassa su fatturato
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+[Comportamento cliente]:
+Nome: Utilizzo del credito
+Tipologia: Positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+Criterio: Queste variabili indicano l'uso attivo del credito da parte del cliente.
+Nome: Rischio di insolvenza
+Tipologia: Negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui), Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+Criterio: Queste variabili indicano un potenziale rischio di insolvenza del cliente.
+[Conclusione]
+Il modello predice la rischiosità del cliente basandosi principalmente su due fattori: l'utilizzo del credito e il rischio di insolvenza. Un utilizzo attivo del credito da parte del cliente è visto come un segnale positivo, mentre segnali di potenziale insolvenza sono visti come negativi. Pertanto, un cliente che utilizza attivamente il suo credito ma mostra segni di potenziale insolvenza sarà considerato più rischioso.</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora in una banca. Il tuo capo ha ricevuto la tabella compresa tra i tag &lt;table&gt; in cui è indicato il contributo ogni variabile alla previsione di un modello di classificazione (Il modello vuole prevedere il rischio di insolvenza di un prestito per un cliente).
+Non essendo una persona tecnica, ha bisogno che lo aiuti ad interpretare la tabella senza riferimenti ai numeri presenti. 
+Ragiona per passi: 
+- Elenca le variabili (massimo 10) con contributo positivo ordinate in maniera decrescente
+- Elenca le variabili (massimo 10) con contributo negativo ordinate in maniera crescente
+- Raggruppa le variabili rilevanti con natura simile e contributo coerente in gruppi. Nomina ciascun gruppo e spiega il significato del gruppo. Utilizza il seguente schema:
+    - Nome: &lt;Nome gruppo&gt;
+    - Tipologia: &lt;contributo positivo o negativo&gt;
+    - Variabili: &lt;Elenco variabili presenti&gt;
+    - Criterio: &lt;Indica il criterio utilizzato per la costruzione del gruppo&gt;
+- Concludi riportando quali gruppi hanno alzato o diminuto il rischio di insolvenza.
+Tieni a mente che un valore positivo di contributo indica che la variabile ha alzato il rischio di insolvenza; valori negativi indicano diminuzione del rischio mentre valori prossimi allo zero indicano scarsa influenza.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Ecco l'interpretazione della tabella:
+Variabili con contributo positivo (ordine decrescente):
+1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+2. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+3. utilizzo su accordato revoca snb
+4. utilizzo su accordato autoliquidante snb
+5. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+7. sconfino medio revoca &gt; 1000€
+8. Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente
+9. utilizzo firma finanziaria su accordato firma finanziaria
+10. Copertura dell'indebitamento
+Variabili con contributo negativo (ordine crescente):
+1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+3. utilizzato cassa su fatturato
+4. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+7. sconfino scadenza su margine scadenza
+8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+Gruppi di variabili rilevanti:
+Nome: Utilizzo del credito
+Tipologia: Contributo positivo
+Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+Criterio: Queste variabili riguardano l'utilizzo del credito da parte del cliente.
+Nome: Sconfino
+Tipologia: Contributo positivo
+Variabili: Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, sconfino medio revoca &gt; 1000€
+Criterio: Queste variabili riguardano il sconfino del cliente.
+Nome: Pagamenti
+Tipologia: Contributo negativo
+Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui), Regolarità mensile nel pagamento di prestiti e finanziamenti
+Criterio: Queste variabili riguardano i pagamenti del cliente.
+In conclusione, i gruppi di variabili che hanno alzato il rischio di insolvenza sono "Utilizzo del credito" e "Sconfino". Il gruppo di variabili che ha diminuito il rischio di insolvenza è "Pagamenti".</t>
+  </si>
+  <si>
+    <t>1 min 5s</t>
+  </si>
+  <si>
+    <t>Sei un data scientist che lavora in una banca. Il tuo capo ha ricevuto la tabella compresa tra i tag &lt;table&gt; in cui è indicato il contributo ogni variabile alla previsione di un modello di classificazione (Il modello vuole prevedere il rischio di insolvenza di un prestito per un cliente).
+Non essendo una persona tecnica, ha bisogno che lo aiuti ad interpretare la tabella senza riferimenti ai numeri presenti. 
+Ragiona per passi: 
+- Elenca le variabili (massimo 10) con contributo positivo ordinate in maniera decrescente
+- Elenca le variabili (massimo 10) con contributo negativo ordinate in maniera crescente
+- Raggruppa le variabili rilevanti con natura simile e contributo coerente in gruppi. Nomina ciascun gruppo e spiega il significato del gruppo. Utilizza il seguente schema:
+    - Nome: &lt;Nome gruppo&gt;
+    - Tipologia: &lt;contributo positivo o negativo&gt;
+    - Variabili: &lt;Elenco variabili presenti&gt;
+    - Criterio: &lt;Indica il criterio utilizzato per la costruzione del gruppo&gt;
+- Concludi riportando quali gruppi hanno alzato o diminuto il rischio di insolvenza ipotizzando il comportamento avuto dal cliente.
+Tieni a mente che un valore positivo di contributo indica che la variabile ha alzato il rischio di insolvenza; valori negativi indicano diminuzione del rischio mentre valori prossimi allo zero indicano scarsa influenza.
+&lt;table&gt;
+| Descrizione                                                                                                     |   importanza |
+|:----------------------------------------------------------------------------------------------------------------|-------------:|
+| Somma Utilizzato su Somma Accordato negli ultimi due mesi                                                       |        0.396 |
+| Media Giorni di Disponibilità CC negli ultimi tre mesi                                                          |        0.098 |
+| Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi                                                 |       -0.1   |
+| Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi                            |        0.257 |
+| Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata                        |        0.207 |
+| Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)                               |       -0.07  |
+| Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi                    |        0.106 |
+| Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi                        |        0.322 |
+| utilizzo su accordato revoca snb                                                                                |        0.308 |
+| utilizzo su accordato autoliquidante snb                                                                        |        0.267 |
+| sconfino scadenza su margine scadenza                                                                           |       -0.002 |
+| utilizzato cassa su fatturato                                                                                   |       -0.033 |
+| factoring scaduto su (factoring pro solvendo + factoring pro soluto)                                            |       -0.022 |
+| sconfino medio revoca &gt; 1000€                                                                                   |        0.183 |
+| utilizzo firma finanziaria su accordato firma finanziaria                                                       |        0.116 |
+| Copertura dell'indebitamento                                                                                    |        0.116 |
+| Debiti bancari su ricavi netti                                                                                  |        0.014 |
+| Valore debiti commerciali                                                                                       |        0.007 |
+| Liquidità su attivo netto                                                                                       |        0.046 |
+| Utile su ricavi                                                                                                 |        0.069 |
+| Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3                                     |       -0.015 |
+| Regolarità mensile nel pagamento di prestiti e finanziamenti                                                    |       -0.001 |
+| Misura di movimentazione del conto, che considera sia il numero che gli importi dei movimenti di conto corrente |        0.174 |
+| Importo mediano della somma entrate settimanali delle ultime 52 settimane                                       |        0.092 |
+| PD media ufficiale nell’ultimo mese                                                                             |        0.261 |
+| Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre                |       -0.027 |
+&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>Ecco un'interpretazione della tabella senza riferimenti ai numeri:
+- Le variabili con contributo positivo, ordinate in maniera decrescente, sono:
+    1. Somma Utilizzato su Somma Accordato negli ultimi due mesi
+    2. Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi
+    3. Somma Importo Effetti Trassati Insoluti su Importo Effetti Scaduti negli ultimi tre mesi
+    4. utilizzo su accordato revoca snb
+    5. utilizzo su accordato autoliquidante snb
+    6. Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata
+    7. sconfino medio revoca &gt; 1000€
+    8. utilizzo firma finanziaria su accordato firma finanziaria
+    9. Copertura dell'indebitamento
+    10. Somma Importo Effetti Protestati + Richiamati su Importo Effetti Scaduti negli ultimi 3 mesi
+- Le variabili con contributo negativo, ordinate in maniera crescente, sono:
+    1. Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi
+    2. Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+    3. factoring scaduto su (factoring pro solvendo + factoring pro soluto)
+    4. utilizzato cassa su fatturato
+    5. Variazione tra il tasso di default previsto a 12 mesi e il tasso osservato nell’ultimo trimestre
+    6. Livello di allerta complessivo, differenziato per Ateco, con soglie 0, 1, 3
+    7. sconfino scadenza su margine scadenza
+    8. Regolarità mensile nel pagamento di prestiti e finanziamenti
+- Raggruppamento delle variabili rilevanti con natura simile e contributo coerente in gruppi:
+    - Nome: Utilizzo del credito
+    - Tipologia: contributo positivo
+    - Variabili: Somma Utilizzato su Somma Accordato negli ultimi due mesi, utilizzo su accordato revoca snb, utilizzo su accordato autoliquidante snb, utilizzo firma finanziaria su accordato firma finanziaria
+    - Criterio: Queste variabili riguardano l'uso del credito da parte del cliente.
+    - Nome: Sconfino
+    - Tipologia: contributo positivo
+    - Variabili: Media pesata per importo del massimo numero giorni di sconfino negli ultimi sei mesi, Flag Massimo Importo Sconfino &gt; 100 nell'ultimo mese - cliente + responsabilità limitata, sconfino medio revoca &gt; 1000€
+    - Criterio: Queste variabili riguardano il superamento del limite di credito da parte del cliente.
+    - Nome: Pagamenti irregolari
+    - Tipologia: contributo negativo
+    - Variabili: Somma Utilizzato su Somma Giacenza Minima negli ultimi due mesi, Massimo Numero di Rate Impagate negli ultimi tre mesi (altro rateali - non mutui)
+    - Criterio: Queste variabili riguardano i pagamenti irregolari o mancati da parte del cliente.
+In conclusione, i gruppi che hanno alzato il rischio di insolvenza sono "Utilizzo del credito" e "Sconfino", che indicano un uso eccessivo del credito e il superamento dei limiti di credito. Il gruppo "Pagamenti irregolari" ha invece diminuito il rischio di insolvenza, indicando che i clienti con pagamenti irregolari o mancati sono meno propensi a diventare insolventi.</t>
+  </si>
 </sst>
 </file>
 
@@ -547,7 +1767,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -570,11 +1790,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,6 +1818,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A2F640-7D2E-454D-A45B-7AFA2AEB1939}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,4 +2311,252 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1634DE-7ED0-42C0-9CF5-E176C72E6799}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="164.1796875" customWidth="1"/>
+    <col min="3" max="3" width="176.453125" customWidth="1"/>
+    <col min="4" max="4" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.36328125" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>